<commit_message>
Fixing Library and Fixing Excel
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0262 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0262 - Searching profiling nasabah & memiliki sales kelolaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A29BD40-431F-48A2-A1DE-DAAFAC83FB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA19EE72-2A9B-4E38-A3C1-8C422529B4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,14 +131,14 @@
 -        Status berubah menjadi disetujui pemimpin</t>
   </si>
   <si>
-    <t>Penyelia SRM</t>
+    <t>Pemimpin Cabang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +170,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -219,6 +226,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +539,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +555,7 @@
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.42578125" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.140625" customWidth="1"/>
@@ -622,7 +633,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="12">
-        <v>20037</v>
+        <v>23320</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>9</v>
@@ -635,13 +646,13 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="12">
-        <v>9003982023</v>
+        <v>10201872811</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="12">
-        <v>9936964558</v>
+      <c r="O2" s="13">
+        <v>9448808661</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="7"/>
@@ -664,8 +675,8 @@
       <c r="E3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="12">
-        <v>37400</v>
+      <c r="F3" s="14">
+        <v>20478</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>9</v>
@@ -697,7 +708,7 @@
         <v>26</v>
       </c>
       <c r="F4" s="12">
-        <v>20037</v>
+        <v>23320</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>9</v>
@@ -716,13 +727,13 @@
         <v>23</v>
       </c>
       <c r="M4" s="12">
-        <v>9003982023</v>
+        <v>10201872811</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="12">
-        <v>9936964558</v>
+      <c r="O4" s="13">
+        <v>9448808661</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="3"/>

</xml_diff>